<commit_message>
Regenerate all formDef.json files, fix imnci_test.xlsx to use daysOld instead of ageDays, remove promptLink functionality from exampleForm.xlsx
</commit_message>
<xml_diff>
--- a/form-files/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/form-files/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="15400" activeTab="2"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="37040" windowHeight="21180"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="158">
   <si>
     <t>type</t>
   </si>
@@ -241,24 +241,6 @@
     <t>Take a picture:</t>
   </si>
   <si>
-    <t>selected(data('examples'), 'prompt_link')</t>
-  </si>
-  <si>
-    <t>&lt;a href="{{promptLink "unreachable"}}"&gt;This is a link to another prompt&lt;/a&gt;</t>
-  </si>
-  <si>
-    <t>goto unreachable_end</t>
-  </si>
-  <si>
-    <t>unreachable</t>
-  </si>
-  <si>
-    <t>This prompt is unreachable except by links.</t>
-  </si>
-  <si>
-    <t>goto prompt_link_return</t>
-  </si>
-  <si>
     <t>selected(data('examples'), 'custom_template')</t>
   </si>
   <si>
@@ -394,12 +376,6 @@
     <t>custom template</t>
   </si>
   <si>
-    <t>prompt_link</t>
-  </si>
-  <si>
-    <t>prompt linking</t>
-  </si>
-  <si>
     <t>sexes</t>
   </si>
   <si>
@@ -452,12 +428,6 @@
   </si>
   <si>
     <t>branch_label</t>
-  </si>
-  <si>
-    <t>prompt_link_return</t>
-  </si>
-  <si>
-    <t>unreachable_end</t>
   </si>
   <si>
     <t>if</t>
@@ -566,18 +536,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9EAD3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -592,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -600,7 +564,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -914,38 +877,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T164"/>
+  <dimension ref="B1:T156"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C75" sqref="C75"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53:XFD53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="2" max="2" width="24.5" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="40.81640625" customWidth="1"/>
-    <col min="5" max="6" width="27.1796875" customWidth="1"/>
-    <col min="7" max="8" width="24.81640625" customWidth="1"/>
-    <col min="9" max="9" width="41.81640625" customWidth="1"/>
+    <col min="4" max="4" width="40.83203125" customWidth="1"/>
+    <col min="5" max="6" width="27.1640625" customWidth="1"/>
+    <col min="7" max="8" width="24.83203125" customWidth="1"/>
+    <col min="9" max="9" width="41.83203125" customWidth="1"/>
     <col min="10" max="10" width="40" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" customWidth="1"/>
+    <col min="11" max="11" width="20.5" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-    <col min="14" max="14" width="18.36328125" customWidth="1"/>
-    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="13" max="13" width="15.83203125" customWidth="1"/>
+    <col min="14" max="14" width="18.33203125" customWidth="1"/>
+    <col min="15" max="15" width="18.5" customWidth="1"/>
     <col min="16" max="16" width="19" customWidth="1"/>
     <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="18.1796875" customWidth="1"/>
-    <col min="20" max="20" width="14.36328125" customWidth="1"/>
+    <col min="19" max="19" width="18.1640625" customWidth="1"/>
+    <col min="20" max="20" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:20" ht="17.5" customHeight="1">
       <c r="B1" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C1" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -953,26 +916,26 @@
       <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>137</v>
+      <c r="F1" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>162</v>
+      <c r="H1" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>5</v>
@@ -996,14 +959,14 @@
         <v>11</v>
       </c>
       <c r="T1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F2" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="2:20" ht="17.5" customHeight="1">
+      <c r="E2" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G2" t="s">
@@ -1013,22 +976,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:20" ht="17.5" customHeight="1">
       <c r="C3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>98</v>
+        <v>136</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="2:20" ht="17.5" customHeight="1">
+      <c r="E4" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="G4" t="s">
         <v>14</v>
@@ -1040,24 +1003,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:20" ht="17.5" customHeight="1">
       <c r="C5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="2:20" ht="17.5" customHeight="1">
       <c r="C6" t="s">
-        <v>143</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="2:20" ht="17.5" customHeight="1">
       <c r="E7" t="s">
         <v>17</v>
       </c>
@@ -1068,7 +1031,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:20" ht="17.5" customHeight="1">
       <c r="E8" t="s">
         <v>19</v>
       </c>
@@ -1079,7 +1042,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:20" ht="17.5" customHeight="1">
       <c r="E9" t="s">
         <v>4</v>
       </c>
@@ -1090,7 +1053,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:20" ht="17.5" customHeight="1">
       <c r="E10" t="s">
         <v>3</v>
       </c>
@@ -1101,24 +1064,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:20" ht="17.5" customHeight="1">
       <c r="C11" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-    </row>
-    <row r="12" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="2:20" ht="17.5" customHeight="1">
       <c r="C12" t="s">
-        <v>143</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="2:20" ht="17.5" customHeight="1">
       <c r="E13" s="1" t="s">
         <v>25</v>
       </c>
@@ -1133,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:20" ht="17.5" customHeight="1">
       <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
@@ -1151,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:20" ht="17.5" customHeight="1">
       <c r="E15" s="1" t="s">
         <v>31</v>
       </c>
@@ -1167,7 +1130,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:20" ht="17.5" customHeight="1">
       <c r="E16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1182,24 +1145,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:20" ht="17.5" customHeight="1">
       <c r="C17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-    </row>
-    <row r="18" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="3:20" ht="17.5" customHeight="1">
       <c r="C18" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D18" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-    </row>
-    <row r="19" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="3:20" ht="17.5" customHeight="1">
       <c r="E19" s="1" t="s">
         <v>36</v>
       </c>
@@ -1211,16 +1174,16 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:20" ht="17.5" customHeight="1">
       <c r="C20" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
-    <row r="21" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:20" ht="17.5" customHeight="1">
       <c r="C21" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D21" t="s">
         <v>37</v>
@@ -1228,26 +1191,26 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:20" ht="17.5" customHeight="1">
       <c r="C22" t="s">
         <v>55</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
-    <row r="23" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="5" t="s">
-        <v>164</v>
+    <row r="23" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E23" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" t="s">
         <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="24" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" ht="17.5" customHeight="1">
       <c r="E24" s="1" t="s">
         <v>36</v>
       </c>
@@ -1259,31 +1222,31 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:20" ht="17.5" customHeight="1">
       <c r="C25" t="s">
         <v>62</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
     </row>
-    <row r="26" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:20" ht="17.5" customHeight="1">
       <c r="C26" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:20" ht="17.5" customHeight="1">
       <c r="C27" t="s">
-        <v>150</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-    </row>
-    <row r="28" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="3:20" ht="17.5" customHeight="1">
       <c r="E28" s="1" t="s">
         <v>42</v>
       </c>
@@ -1295,9 +1258,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:20" ht="17.5" customHeight="1">
       <c r="C29" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D29" t="s">
         <v>45</v>
@@ -1306,7 +1269,7 @@
       <c r="F29" s="1"/>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:20" ht="17.5" customHeight="1">
       <c r="E30" s="1" t="s">
         <v>25</v>
       </c>
@@ -1321,15 +1284,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:20" ht="17.5" customHeight="1">
       <c r="C31" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:20" ht="17.5" customHeight="1">
       <c r="E32" s="1" t="s">
         <v>48</v>
       </c>
@@ -1341,7 +1304,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" ht="17.5" customHeight="1">
       <c r="E33" s="1" t="s">
         <v>50</v>
       </c>
@@ -1354,28 +1317,28 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" ht="17.5" customHeight="1">
       <c r="C34" t="s">
-        <v>151</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
+        <v>141</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" ht="17.5" customHeight="1">
       <c r="C35" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9" ht="17.5" customHeight="1">
       <c r="E36" s="1" t="s">
         <v>19</v>
       </c>
@@ -1388,9 +1351,9 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9" ht="17.5" customHeight="1">
       <c r="C37" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -1398,9 +1361,9 @@
       <c r="H37" s="1"/>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9" ht="17.5" customHeight="1">
       <c r="C38" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D38" t="s">
         <v>56</v>
@@ -1411,18 +1374,18 @@
       <c r="H38" s="1"/>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:9" ht="17.5" customHeight="1">
       <c r="C39" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F39" s="1"/>
     </row>
-    <row r="40" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E40" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>101</v>
+    <row r="40" spans="3:9" ht="17.5" customHeight="1">
+      <c r="E40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>95</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>57</v>
@@ -1432,25 +1395,25 @@
         <v>58</v>
       </c>
     </row>
-    <row r="41" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:9" ht="17.5" customHeight="1">
       <c r="C41" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E42" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F42" s="5" t="s">
-        <v>98</v>
+    <row r="42" spans="3:9" ht="17.5" customHeight="1">
+      <c r="E42" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>92</v>
       </c>
       <c r="G42" s="1" t="s">
         <v>60</v>
@@ -1460,46 +1423,46 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9" ht="17.5" customHeight="1">
       <c r="C43" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9" ht="17.5" customHeight="1">
       <c r="C44" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F44" s="1"/>
     </row>
-    <row r="45" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C45" s="5" t="s">
-        <v>157</v>
+    <row r="45" spans="3:9" ht="17.5" customHeight="1">
+      <c r="C45" s="4" t="s">
+        <v>147</v>
       </c>
       <c r="F45" s="1"/>
     </row>
-    <row r="46" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9" ht="17.5" customHeight="1">
       <c r="C46" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="D46" t="s">
-        <v>155</v>
-      </c>
-      <c r="E46" s="8"/>
-      <c r="F46" s="8"/>
-    </row>
-    <row r="47" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="3:9" ht="17.5" customHeight="1">
       <c r="C47" s="1" t="s">
         <v>55</v>
       </c>
       <c r="F47" s="1"/>
     </row>
-    <row r="48" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:9" ht="17.5" customHeight="1">
       <c r="E48" s="1" t="s">
         <v>3</v>
       </c>
@@ -1512,7 +1475,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="49" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:20" ht="17.5" customHeight="1">
       <c r="E49" s="1" t="s">
         <v>65</v>
       </c>
@@ -1525,7 +1488,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="50" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:20" ht="17.5" customHeight="1">
       <c r="E50" s="1" t="s">
         <v>4</v>
       </c>
@@ -1538,358 +1501,280 @@
         <v>69</v>
       </c>
     </row>
-    <row r="51" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:20" ht="17.5" customHeight="1">
       <c r="C51" s="1" t="s">
         <v>62</v>
       </c>
       <c r="F51" s="1"/>
     </row>
-    <row r="52" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:20" ht="17.5" customHeight="1">
       <c r="C52" t="s">
-        <v>144</v>
-      </c>
-      <c r="E52" s="6"/>
-      <c r="F52" s="6"/>
+        <v>134</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5"/>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:20" ht="17.5" customHeight="1">
       <c r="C53" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="D53" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
+    <row r="54" spans="3:20" ht="17.5" customHeight="1">
+      <c r="C54" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F54" s="1"/>
+      <c r="I54" s="2"/>
+    </row>
+    <row r="55" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E55" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F54" s="1"/>
-      <c r="I54" s="2" t="s">
+      <c r="F55" s="1"/>
+      <c r="I55" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="T54" t="b">
+      <c r="T55" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
-        <v>144</v>
-      </c>
-      <c r="E55" s="1"/>
-      <c r="F55" s="1"/>
-      <c r="I55" s="2"/>
-    </row>
-    <row r="56" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>141</v>
-      </c>
-      <c r="E56" s="6"/>
-      <c r="F56" s="6"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C57" s="3" t="s">
+    <row r="56" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E56" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F56" s="1"/>
+      <c r="G56" t="s">
         <v>72</v>
       </c>
-      <c r="E57" s="7"/>
-      <c r="F57" s="8"/>
-      <c r="I57" s="2"/>
-    </row>
-    <row r="58" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E58" s="1" t="s">
+      <c r="I56" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J56" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q56" t="s">
+        <v>75</v>
+      </c>
+      <c r="R56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E57" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="1"/>
+      <c r="G57" t="s">
+        <v>78</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="58" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E58" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G58" t="s">
+        <v>80</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="59" spans="3:20" ht="17.5" customHeight="1">
+      <c r="C59" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F59" s="1"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E60" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F58" s="1"/>
-      <c r="G58" t="s">
-        <v>73</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="T58" t="b">
+      <c r="F60" s="1"/>
+      <c r="G60" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H60" s="1"/>
+      <c r="I60" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="M60" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T60" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="E59" s="7"/>
-      <c r="F59" s="8"/>
-      <c r="I59" s="2"/>
-    </row>
-    <row r="60" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>142</v>
-      </c>
-      <c r="E60" s="6"/>
-      <c r="F60" s="6"/>
-      <c r="I60" s="2"/>
-    </row>
-    <row r="61" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:20" ht="17.5" customHeight="1">
       <c r="C61" t="s">
-        <v>143</v>
-      </c>
-      <c r="D61" t="s">
-        <v>76</v>
-      </c>
-      <c r="E61" s="6"/>
-      <c r="F61" s="6"/>
+        <v>134</v>
+      </c>
+      <c r="E61" s="1"/>
+      <c r="F61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="1"/>
       <c r="I61" s="2"/>
-    </row>
-    <row r="62" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C62" s="1" t="s">
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="3:20" ht="17.5" customHeight="1">
+      <c r="C62" t="s">
         <v>55</v>
       </c>
+      <c r="E62" s="1"/>
       <c r="F62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="1"/>
       <c r="I62" s="2"/>
-    </row>
-    <row r="63" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E63" s="1" t="s">
-        <v>25</v>
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="3:20" ht="17.5" customHeight="1">
+      <c r="E63" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="F63" s="1"/>
-      <c r="I63" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="T63" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="64" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G63" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I63" s="2"/>
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="3:20" ht="17.5" customHeight="1">
       <c r="E64" s="1" t="s">
         <v>36</v>
       </c>
       <c r="F64" s="1"/>
-      <c r="G64" t="s">
-        <v>78</v>
-      </c>
+      <c r="G64" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H64" s="1"/>
       <c r="I64" s="2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="J64" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q64" t="s">
-        <v>81</v>
-      </c>
-      <c r="R64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E65" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="F65" s="1"/>
-      <c r="G65" t="s">
-        <v>84</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="66" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E66" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="F66" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="G66" t="s">
-        <v>86</v>
-      </c>
-      <c r="I66" s="2" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="67" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C67" s="1" t="s">
+      <c r="N64" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="O64" s="1">
+        <v>1</v>
+      </c>
+      <c r="P64" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" ht="17.5" customHeight="1">
+      <c r="C65" t="s">
         <v>62</v>
       </c>
-      <c r="F67" s="1"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E68" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F68" s="1"/>
-      <c r="G68" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H68" s="1"/>
-      <c r="I68" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M68" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="T68" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>144</v>
-      </c>
-      <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
-      <c r="G69" s="1"/>
-      <c r="H69" s="1"/>
-      <c r="I69" s="2"/>
-      <c r="M69" s="1"/>
-    </row>
-    <row r="70" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>55</v>
-      </c>
-      <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
-      <c r="G70" s="1"/>
-      <c r="H70" s="1"/>
-      <c r="I70" s="2"/>
-      <c r="M70" s="1"/>
-    </row>
-    <row r="71" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E71" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F71" s="1"/>
-      <c r="G71" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="H71" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="I71" s="2"/>
-      <c r="M71" s="1"/>
-    </row>
-    <row r="72" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E72" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F72" s="1"/>
-      <c r="G72" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="H72" s="1"/>
-      <c r="I72" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="J72" t="s">
-        <v>93</v>
-      </c>
-      <c r="N72" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="O72" s="1">
-        <v>1</v>
-      </c>
-      <c r="P72" s="1">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="66" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="67" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="68" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="69" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="70" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="71" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="72" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="73" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="74" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="75" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="76" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="77" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="78" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="79" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="80" spans="3:3" ht="17.5" customHeight="1"/>
+    <row r="81" ht="17.5" customHeight="1"/>
+    <row r="82" ht="17.5" customHeight="1"/>
+    <row r="83" ht="17.5" customHeight="1"/>
+    <row r="84" ht="17.5" customHeight="1"/>
+    <row r="85" ht="17.5" customHeight="1"/>
+    <row r="86" ht="17.5" customHeight="1"/>
+    <row r="87" ht="17.5" customHeight="1"/>
+    <row r="88" ht="17.5" customHeight="1"/>
+    <row r="89" ht="17.5" customHeight="1"/>
+    <row r="90" ht="17.5" customHeight="1"/>
+    <row r="91" ht="17.5" customHeight="1"/>
+    <row r="92" ht="17.5" customHeight="1"/>
+    <row r="93" ht="17.5" customHeight="1"/>
+    <row r="94" ht="17.5" customHeight="1"/>
+    <row r="95" ht="17.5" customHeight="1"/>
+    <row r="96" ht="17.5" customHeight="1"/>
+    <row r="97" ht="17.5" customHeight="1"/>
+    <row r="98" ht="17.5" customHeight="1"/>
+    <row r="99" ht="17.5" customHeight="1"/>
+    <row r="100" ht="17.5" customHeight="1"/>
+    <row r="101" ht="17.5" customHeight="1"/>
+    <row r="102" ht="17.5" customHeight="1"/>
+    <row r="103" ht="17.5" customHeight="1"/>
+    <row r="104" ht="17.5" customHeight="1"/>
+    <row r="105" ht="17.5" customHeight="1"/>
+    <row r="106" ht="17.5" customHeight="1"/>
+    <row r="107" ht="17.5" customHeight="1"/>
+    <row r="108" ht="17.5" customHeight="1"/>
+    <row r="109" ht="17.5" customHeight="1"/>
+    <row r="110" ht="17.5" customHeight="1"/>
+    <row r="111" ht="17.5" customHeight="1"/>
+    <row r="112" ht="17.5" customHeight="1"/>
+    <row r="113" ht="17.5" customHeight="1"/>
+    <row r="114" ht="17.5" customHeight="1"/>
+    <row r="115" ht="17.5" customHeight="1"/>
+    <row r="116" ht="17.5" customHeight="1"/>
+    <row r="117" ht="17.5" customHeight="1"/>
+    <row r="118" ht="17.5" customHeight="1"/>
+    <row r="119" ht="17.5" customHeight="1"/>
+    <row r="120" ht="17.5" customHeight="1"/>
+    <row r="121" ht="17.5" customHeight="1"/>
+    <row r="122" ht="17.5" customHeight="1"/>
+    <row r="123" ht="17.5" customHeight="1"/>
+    <row r="124" ht="17.5" customHeight="1"/>
+    <row r="125" ht="17.5" customHeight="1"/>
+    <row r="126" ht="17.5" customHeight="1"/>
+    <row r="127" ht="17.5" customHeight="1"/>
+    <row r="128" ht="17.5" customHeight="1"/>
+    <row r="129" ht="17.5" customHeight="1"/>
+    <row r="130" ht="17.5" customHeight="1"/>
+    <row r="131" ht="17.5" customHeight="1"/>
+    <row r="132" ht="17.5" customHeight="1"/>
+    <row r="133" ht="17.5" customHeight="1"/>
+    <row r="134" ht="17.5" customHeight="1"/>
+    <row r="135" ht="17.5" customHeight="1"/>
+    <row r="136" ht="17.5" customHeight="1"/>
+    <row r="137" ht="17.5" customHeight="1"/>
+    <row r="138" ht="17.5" customHeight="1"/>
+    <row r="139" ht="17.5" customHeight="1"/>
+    <row r="140" ht="17.5" customHeight="1"/>
+    <row r="141" ht="17.5" customHeight="1"/>
+    <row r="142" ht="17.5" customHeight="1"/>
+    <row r="143" ht="17.5" customHeight="1"/>
+    <row r="144" ht="17.5" customHeight="1"/>
+    <row r="145" ht="17.5" customHeight="1"/>
+    <row r="146" ht="17.5" customHeight="1"/>
+    <row r="147" ht="17.5" customHeight="1"/>
+    <row r="148" ht="17.5" customHeight="1"/>
+    <row r="149" ht="17.5" customHeight="1"/>
+    <row r="150" ht="17.5" customHeight="1"/>
+    <row r="151" ht="17.5" customHeight="1"/>
+    <row r="152" ht="17.5" customHeight="1"/>
+    <row r="153" ht="17.5" customHeight="1"/>
+    <row r="154" ht="17.5" customHeight="1"/>
+    <row r="155" ht="17.5" customHeight="1"/>
+    <row r="156" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1908,26 +1793,26 @@
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.453125" customWidth="1"/>
-    <col min="2" max="2" width="49.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="49.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>135</v>
+    <row r="1" spans="1:2" ht="17.5" customHeight="1">
+      <c r="A1" s="4" t="s">
+        <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1942,164 +1827,164 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="17.5" customHeight="1">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="17.5" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="7" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A7" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C7" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A8" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C8" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A9" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C9" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A10" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>110</v>
-      </c>
       <c r="C10" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="12" spans="1:3" ht="17.5" customHeight="1">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C12" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="17.5" customHeight="1">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="17.5" customHeight="1">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="17.5" customHeight="1">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -2110,7 +1995,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17.5" customHeight="1">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -2121,75 +2006,64 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="17.5" customHeight="1">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17.5" customHeight="1">
       <c r="A18" t="s">
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="17.5" customHeight="1">
       <c r="A19" t="s">
         <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="21" spans="1:3" ht="17.5" customHeight="1">
+      <c r="A21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="17.5" customHeight="1">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>123</v>
-      </c>
-      <c r="B23" t="s">
-        <v>125</v>
-      </c>
-      <c r="C23" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:3" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.5" customHeight="1"/>
+    <row r="24" spans="1:3" ht="17.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2208,51 +2082,51 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1"/>
-    <col min="2" max="2" width="24.1796875" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5" customWidth="1"/>
+    <col min="2" max="2" width="24.1640625" customWidth="1"/>
+    <col min="3" max="3" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
-        <v>132</v>
+    <row r="1" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A1" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C1" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="14.5" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="14.5" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1">
         <v>20130408</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>159</v>
+    <row r="4" spans="1:3" ht="14.5" customHeight="1">
+      <c r="A4" s="4" t="s">
+        <v>149</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="6" spans="1:3" ht="14.5" customHeight="1"/>
+    <row r="7" spans="1:3" ht="14.5" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Updated ExampleForm using a session variable.
</commit_message>
<xml_diff>
--- a/form-files/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
+++ b/form-files/tables/exampleForm/forms/exampleForm/exampleForm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="6360" windowWidth="25820" windowHeight="16220"/>
+    <workbookView xWindow="1920" yWindow="6360" windowWidth="19420" windowHeight="12220"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="156">
   <si>
     <t>type</t>
   </si>
@@ -481,10 +481,22 @@
     <t>(( data('coffee_today') == null ) ? data('avg_coffee') : data('coffee_today'))</t>
   </si>
   <si>
-    <t>((data('rating') == null) ? 5 : data('rating'))</t>
-  </si>
-  <si>
     <t>computed assignment of initial values</t>
+  </si>
+  <si>
+    <t>model.isSessionVariable</t>
+  </si>
+  <si>
+    <t>((data('rating') == null) ? data('default_rating') : data('rating'))</t>
+  </si>
+  <si>
+    <t>default_rating</t>
+  </si>
+  <si>
+    <t>Enter an initial rating (1-10) for this survey</t>
+  </si>
+  <si>
+    <t>If the form does not yet have a rating, this will be proposed for the rating value.  This value is not retained in the survey result set and exists only for the duration of this survey session.</t>
   </si>
 </sst>
 </file>
@@ -859,10 +871,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:T153"/>
+  <dimension ref="B1:U154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -872,20 +884,20 @@
     <col min="4" max="4" width="40.81640625" customWidth="1"/>
     <col min="5" max="6" width="27.1796875" customWidth="1"/>
     <col min="7" max="8" width="24.81640625" customWidth="1"/>
-    <col min="9" max="9" width="41.81640625" customWidth="1"/>
-    <col min="10" max="10" width="40" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" customWidth="1"/>
-    <col min="12" max="12" width="13" customWidth="1"/>
-    <col min="13" max="13" width="15.81640625" customWidth="1"/>
-    <col min="14" max="14" width="18.36328125" customWidth="1"/>
-    <col min="15" max="15" width="18.453125" customWidth="1"/>
-    <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="18" max="18" width="16" customWidth="1"/>
-    <col min="19" max="19" width="18.1796875" customWidth="1"/>
-    <col min="20" max="20" width="14.36328125" customWidth="1"/>
+    <col min="9" max="10" width="41.81640625" customWidth="1"/>
+    <col min="11" max="11" width="40" customWidth="1"/>
+    <col min="12" max="12" width="20.453125" customWidth="1"/>
+    <col min="13" max="13" width="13" customWidth="1"/>
+    <col min="14" max="14" width="15.81640625" customWidth="1"/>
+    <col min="15" max="15" width="18.36328125" customWidth="1"/>
+    <col min="16" max="16" width="18.453125" customWidth="1"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
+    <col min="19" max="19" width="16" customWidth="1"/>
+    <col min="20" max="20" width="18.1796875" customWidth="1"/>
+    <col min="21" max="21" width="14.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>129</v>
       </c>
@@ -910,730 +922,782 @@
       <c r="I1" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" t="s">
+        <v>153</v>
+      </c>
+      <c r="I2" t="s">
+        <v>154</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="4" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
+    <row r="6" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G6" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
+    <row r="7" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
         <v>4</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G7" t="s">
         <v>18</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" t="s">
+    <row r="8" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G8" t="s">
         <v>20</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>131</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-    </row>
-    <row r="10" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="I10" t="s">
-        <v>23</v>
-      </c>
-      <c r="J10" t="s">
-        <v>24</v>
-      </c>
-      <c r="T10" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>22</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="I11" s="2" t="s">
+      <c r="I11" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" t="s">
+        <v>24</v>
+      </c>
+      <c r="U11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="I12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="J12" s="2"/>
+      <c r="L12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="M12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="T11" t="b">
+      <c r="U12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E12" s="1" t="s">
+    <row r="13" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1" t="s">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H12" s="1"/>
-      <c r="I12" s="2" t="s">
+      <c r="H13" s="1"/>
+      <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J13" s="2"/>
+      <c r="K13" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E13" s="1" t="s">
+    <row r="14" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="I13" s="2" t="s">
+      <c r="F14" s="1"/>
+      <c r="I14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" s="2"/>
+      <c r="K14" t="s">
         <v>32</v>
       </c>
-      <c r="T13" t="b">
+      <c r="U14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>131</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="2:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E16" s="1" t="s">
+    <row r="16" spans="2:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>130</v>
+      </c>
+      <c r="D16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="1"/>
-      <c r="G16" t="s">
+      <c r="F17" s="1"/>
+      <c r="G17" t="s">
         <v>35</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+    <row r="18" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
         <v>131</v>
-      </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>130</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
-    <row r="19" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>52</v>
+        <v>130</v>
+      </c>
+      <c r="D19" t="s">
+        <v>34</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
-    <row r="20" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="4" t="s">
+    <row r="20" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E21" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="F20" s="1"/>
-      <c r="G20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H20" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="21" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" t="s">
         <v>37</v>
       </c>
-      <c r="I21" t="s">
+      <c r="H21" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="22" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" s="1"/>
+      <c r="G22" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
         <v>59</v>
-      </c>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>131</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="24" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
         <v>134</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-    </row>
-    <row r="25" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="1" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F25" s="1"/>
-      <c r="G25" t="s">
+      <c r="F26" s="1"/>
+      <c r="G26" t="s">
         <v>40</v>
       </c>
-      <c r="I25" s="2" t="s">
+      <c r="I26" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="26" spans="3:20" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="J26" s="2"/>
+    </row>
+    <row r="27" spans="3:21" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
         <v>130</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>42</v>
       </c>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E27" s="1" t="s">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+    </row>
+    <row r="28" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="1"/>
-      <c r="I27" s="2" t="s">
+      <c r="F28" s="1"/>
+      <c r="I28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J28" s="2"/>
+      <c r="K28" t="s">
         <v>44</v>
       </c>
-      <c r="T27" t="b">
+      <c r="U28" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E29" s="1" t="s">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+    </row>
+    <row r="30" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F29" s="1"/>
-      <c r="G29" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" t="s">
         <v>45</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I30" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="30" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="1" t="s">
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1" t="s">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="2" t="s">
+      <c r="H31" s="1"/>
+      <c r="I31" s="2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="31" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="J31" s="2"/>
+    </row>
+    <row r="32" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
         <v>135</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="32" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
-        <v>130</v>
-      </c>
-      <c r="D32" t="s">
-        <v>49</v>
       </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="1" t="s">
+    <row r="33" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1" t="s">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="2" t="s">
+      <c r="H34" s="1"/>
+      <c r="I34" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="34" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C34" t="s">
+      <c r="J34" s="2"/>
+    </row>
+    <row r="35" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
         <v>136</v>
-      </c>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="2"/>
-    </row>
-    <row r="35" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" t="s">
-        <v>137</v>
-      </c>
-      <c r="D35" t="s">
-        <v>53</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="2"/>
-    </row>
-    <row r="36" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="1" t="s">
+      <c r="J35" s="2"/>
+    </row>
+    <row r="36" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>137</v>
+      </c>
+      <c r="D36" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+    </row>
+    <row r="37" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F36" s="1"/>
-    </row>
-    <row r="37" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E37" s="4" t="s">
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F38" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="G37" s="1" t="s">
+      <c r="G38" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="2" t="s">
+      <c r="H38" s="1"/>
+      <c r="I38" s="2" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="38" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C38" t="s">
+      <c r="J38" s="2"/>
+    </row>
+    <row r="39" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
         <v>130</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="D39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="1"/>
-      <c r="H38" s="1"/>
-      <c r="I38" s="2"/>
-    </row>
-    <row r="39" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E39" s="4" t="s">
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+    </row>
+    <row r="40" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="F40" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G40" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="2" t="s">
+      <c r="H40" s="1"/>
+      <c r="I40" s="2" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="40" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+      <c r="J40" s="2"/>
+    </row>
+    <row r="41" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
         <v>131</v>
       </c>
-      <c r="D40" s="1"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="1"/>
-      <c r="H40" s="1"/>
-      <c r="I40" s="2"/>
-    </row>
-    <row r="41" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
+      <c r="D41" s="1"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="2"/>
+    </row>
+    <row r="42" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C42" s="4" t="s">
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C43" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C43" t="s">
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
         <v>138</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D44" t="s">
         <v>139</v>
       </c>
-      <c r="E43" s="7"/>
-      <c r="F43" s="7"/>
-    </row>
-    <row r="44" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+    </row>
+    <row r="45" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F44" s="1"/>
-    </row>
-    <row r="45" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H45" s="1"/>
-      <c r="I45" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="46" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E46" s="1" t="s">
-        <v>62</v>
       </c>
       <c r="F46" s="1"/>
       <c r="G46" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+      <c r="J46" s="2"/>
+    </row>
+    <row r="47" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E47" s="1" t="s">
-        <v>4</v>
+        <v>62</v>
       </c>
       <c r="F47" s="1"/>
       <c r="G47" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H47" s="1"/>
       <c r="I47" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J47" s="2"/>
+    </row>
+    <row r="48" spans="3:10" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E48" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H48" s="1"/>
+      <c r="I48" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="48" spans="3:9" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C48" s="1" t="s">
+      <c r="J48" s="2"/>
+    </row>
+    <row r="49" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
         <v>131</v>
-      </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="I49" s="2"/>
-    </row>
-    <row r="50" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" t="s">
-        <v>67</v>
       </c>
       <c r="E50" s="5"/>
       <c r="F50" s="5"/>
       <c r="I50" s="2"/>
-    </row>
-    <row r="51" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="1" t="s">
+      <c r="J50" s="2"/>
+    </row>
+    <row r="51" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>130</v>
+      </c>
+      <c r="D51" t="s">
+        <v>67</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="I51" s="2"/>
+      <c r="J51" s="2"/>
+    </row>
+    <row r="52" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F51" s="1"/>
-      <c r="I51" s="2"/>
-    </row>
-    <row r="52" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E52" s="1" t="s">
+      <c r="F52" s="1"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+    </row>
+    <row r="53" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F52" s="1"/>
-      <c r="I52" s="2" t="s">
+      <c r="F53" s="1"/>
+      <c r="I53" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="T52" t="b">
+      <c r="J53" s="2"/>
+      <c r="U53" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E53" s="1" t="s">
+    <row r="54" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="F53" s="1"/>
-      <c r="G53" t="s">
-        <v>69</v>
-      </c>
-      <c r="I53" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J53" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q53" t="s">
-        <v>72</v>
-      </c>
-      <c r="R53" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E54" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F54" s="1"/>
       <c r="G54" t="s">
+        <v>69</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J54" s="2"/>
+      <c r="K54" t="s">
+        <v>71</v>
+      </c>
+      <c r="R54" t="s">
+        <v>72</v>
+      </c>
+      <c r="S54" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" s="1"/>
+      <c r="G55" t="s">
         <v>75</v>
       </c>
-      <c r="I54" s="2" t="s">
+      <c r="I55" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="55" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E55" s="4" t="s">
+      <c r="J55" s="2"/>
+    </row>
+    <row r="56" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="F55" s="4" t="s">
+      <c r="F56" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="G55" t="s">
+      <c r="G56" t="s">
         <v>77</v>
       </c>
-      <c r="I55" s="2" t="s">
+      <c r="I56" s="2" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="56" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C56" s="1" t="s">
+      <c r="J56" s="2"/>
+    </row>
+    <row r="57" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F56" s="1"/>
-      <c r="I56" s="2"/>
-    </row>
-    <row r="57" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E57" s="1" t="s">
+      <c r="F57" s="1"/>
+      <c r="I57" s="2"/>
+      <c r="J57" s="2"/>
+    </row>
+    <row r="58" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F57" s="1"/>
-      <c r="G57" s="1" t="s">
+      <c r="F58" s="1"/>
+      <c r="G58" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="H57" s="1"/>
-      <c r="I57" s="2" t="s">
+      <c r="H58" s="1"/>
+      <c r="I58" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="M57" s="1" t="s">
+      <c r="J58" s="2"/>
+      <c r="N58" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="T57" t="b">
+      <c r="U58" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C58" t="s">
+    <row r="59" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
         <v>131</v>
-      </c>
-      <c r="E58" s="1"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="1"/>
-      <c r="H58" s="1"/>
-      <c r="I58" s="2"/>
-      <c r="M58" s="1"/>
-    </row>
-    <row r="59" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C59" t="s">
-        <v>52</v>
       </c>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
       <c r="H59" s="1"/>
       <c r="I59" s="2"/>
-      <c r="M59" s="1"/>
-    </row>
-    <row r="60" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E60" s="4" t="s">
+      <c r="J59" s="2"/>
+      <c r="N59" s="1"/>
+    </row>
+    <row r="60" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>52</v>
+      </c>
+      <c r="E60" s="1"/>
+      <c r="F60" s="1"/>
+      <c r="G60" s="1"/>
+      <c r="H60" s="1"/>
+      <c r="I60" s="2"/>
+      <c r="J60" s="2"/>
+      <c r="N60" s="1"/>
+    </row>
+    <row r="61" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E61" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="F60" s="1"/>
-      <c r="G60" s="4" t="s">
+      <c r="F61" s="1"/>
+      <c r="G61" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="H60" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="I60" s="2"/>
-      <c r="M60" s="1"/>
-    </row>
-    <row r="61" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E61" s="1" t="s">
+      <c r="H61" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="I61" s="2"/>
+      <c r="J61" s="2"/>
+      <c r="N61" s="1"/>
+    </row>
+    <row r="62" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E62" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F61" s="1"/>
-      <c r="G61" s="1" t="s">
+      <c r="F62" s="1"/>
+      <c r="G62" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="H61" s="1"/>
-      <c r="I61" s="2" t="s">
+      <c r="H62" s="1"/>
+      <c r="I62" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J62" s="2"/>
+      <c r="K62" t="s">
         <v>84</v>
       </c>
-      <c r="N61" s="1" t="s">
+      <c r="O62" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="O61" s="1">
+      <c r="P62" s="1">
         <v>1</v>
       </c>
-      <c r="P61" s="1">
+      <c r="Q62" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="62" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C62" t="s">
+    <row r="63" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" spans="3:20" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="3:21" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="65" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="66" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="67" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1723,6 +1787,7 @@
     <row r="151" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="152" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="153" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="17.5" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1929,7 +1994,7 @@
         <v>106</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>